<commit_message>
rbs 7 images added
</commit_message>
<xml_diff>
--- a/RBS_7Setembro/RBS_07Setembro.xlsx
+++ b/RBS_7Setembro/RBS_07Setembro.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7260" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Runs" sheetId="2" r:id="rId2"/>
+    <sheet name="Runs" sheetId="2" r:id="rId1"/>
+    <sheet name="Ta-Nb-V Calib." sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Run</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>Au 2</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Nb</t>
+  </si>
+  <si>
+    <t>Ta</t>
+  </si>
+  <si>
+    <t>170 º</t>
+  </si>
+  <si>
+    <t>160 º</t>
+  </si>
+  <si>
+    <t>Mean K factor</t>
   </si>
 </sst>
 </file>
@@ -457,40 +475,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B5"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B3">
-        <f>0.000015*6.022E+23*3.18/78.07</f>
-        <v>3.6793826053541702E+17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B5">
-        <f>0.0015*6.022E+23*1.23/100.117</f>
-        <v>1.1097605801212582E+19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -761,4 +748,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
review TaNbV calib on next commit
</commit_message>
<xml_diff>
--- a/RBS_7Setembro/RBS_07Setembro.xlsx
+++ b/RBS_7Setembro/RBS_07Setembro.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Runs" sheetId="2" r:id="rId1"/>
     <sheet name="Ta-Nb-V Calib." sheetId="3" r:id="rId2"/>
     <sheet name="YbGeSiO Calib." sheetId="4" r:id="rId3"/>
+    <sheet name="Stop. Powers" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>Run</t>
   </si>
@@ -161,6 +162,24 @@
   </si>
   <si>
     <t xml:space="preserve">*Ch + </t>
+  </si>
+  <si>
+    <t>Layer nr</t>
+  </si>
+  <si>
+    <t>Effective E</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>Density (g cm-3)</t>
   </si>
 </sst>
 </file>
@@ -303,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -365,11 +384,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -469,6 +497,9 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,11 +735,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1356749824"/>
-        <c:axId val="-1356744384"/>
+        <c:axId val="-2007904304"/>
+        <c:axId val="-2007903216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1356749824"/>
+        <c:axId val="-2007904304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,12 +852,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1356744384"/>
+        <c:crossAx val="-2007903216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1356744384"/>
+        <c:axId val="-2007903216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,7 +970,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1356749824"/>
+        <c:crossAx val="-2007904304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1035,6 +1066,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1200,11 +1232,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1356742752"/>
-        <c:axId val="-1356737312"/>
+        <c:axId val="-2007916272"/>
+        <c:axId val="-2007914096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1356742752"/>
+        <c:axId val="-2007916272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,6 +1282,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1316,12 +1349,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1356737312"/>
+        <c:crossAx val="-2007914096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1356737312"/>
+        <c:axId val="-2007914096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -1369,6 +1402,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1435,7 +1469,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1356742752"/>
+        <c:crossAx val="-2007916272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3250,10 +3284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3262,7 +3296,7 @@
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="40" t="s">
         <v>26</v>
       </c>
@@ -3273,7 +3307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
@@ -3286,8 +3320,20 @@
       <c r="F3" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H3" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="39">
+        <v>0.71840000000000004</v>
+      </c>
+      <c r="J3" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="39">
+        <v>-1448.4422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" s="33" t="s">
         <v>39</v>
       </c>
@@ -3305,8 +3351,16 @@
         <f t="shared" ref="F4:F8" si="1">$B$1*E4</f>
         <v>1555.4999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H4" s="38"/>
+      <c r="I4" s="38">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38">
+        <v>60.503700000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" s="23" t="s">
         <v>38</v>
       </c>
@@ -3325,7 +3379,7 @@
         <v>1733.4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" s="23"/>
       <c r="C6" s="23">
         <v>0.86580000000000001</v>
@@ -3342,7 +3396,7 @@
         <v>1732.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" s="23"/>
       <c r="C7" s="23">
         <v>0.87009999999999998</v>
@@ -3359,7 +3413,7 @@
         <v>1741.1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" s="23"/>
       <c r="C8" s="23">
         <v>0.87409999999999999</v>
@@ -3376,7 +3430,7 @@
         <v>1749.1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
@@ -3395,7 +3449,7 @@
         <v>1850.6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B10" s="7"/>
       <c r="C10" s="11">
         <v>0.92300000000000004</v>
@@ -3413,7 +3467,7 @@
       </c>
       <c r="J10" s="27"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>21</v>
       </c>
@@ -3432,7 +3486,7 @@
         <v>1916.7</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
@@ -3451,7 +3505,7 @@
         <v>1956.7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" s="9"/>
       <c r="C13" s="13">
         <v>0.97799999999999998</v>
@@ -3468,7 +3522,7 @@
         <v>1956.5000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="9"/>
       <c r="C14" s="9">
         <v>0.97809999999999997</v>
@@ -3485,8 +3539,8 @@
         <v>1956.7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="15" t="s">
         <v>29</v>
       </c>
@@ -3517,8 +3571,14 @@
       <c r="K17" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L17" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="M17" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
@@ -3553,20 +3613,11 @@
         <f>F14</f>
         <v>1956.7</v>
       </c>
-      <c r="M18" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="N18" s="39">
-        <v>0.71840000000000004</v>
-      </c>
-      <c r="O18" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="P18" s="39">
-        <v>-1448.4422</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
         <v>21</v>
       </c>
@@ -3601,16 +3652,11 @@
         <f>F11</f>
         <v>1916.7</v>
       </c>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38">
-        <v>1.8200000000000001E-2</v>
-      </c>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38">
-        <v>60.503700000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>20</v>
       </c>
@@ -3645,8 +3691,15 @@
         <f>F9</f>
         <v>1850.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <f>F9</f>
+        <v>1850.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
         <v>38</v>
       </c>
@@ -3661,7 +3714,7 @@
         <v>1733.4</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="33" t="s">
         <v>39</v>
       </c>
@@ -3688,7 +3741,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3820,4 +3873,41 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>